<commit_message>
adding Program related test data
</commit_message>
<xml_diff>
--- a/TestData/excelData.xlsx
+++ b/TestData/excelData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samee\Work\Projects\Team14_Selenium_Samurai_LMS_Feb2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumod\git\Team14_Selenium_Samurai_LMS_Feb2025\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF83A9A3-E797-468A-847D-3F775435A618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36A09F5-A532-4ECA-B118-177744B2D613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2198BB61-55EA-408D-B3CF-1475E78217FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2198BB61-55EA-408D-B3CF-1475E78217FD}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>sdetnumpyninja@gmail.com</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>You are logged in</t>
+  </si>
+  <si>
+    <t>Programname</t>
+  </si>
+  <si>
+    <t>Programdescription</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>CoreJavaProgrammingLeven</t>
   </si>
 </sst>
 </file>
@@ -485,20 +497,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80ED2E-AA63-4AC9-BD7E-7D4B9BDB8A53}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.36328125" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -515,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,126 +544,126 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -673,7 +685,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -681,12 +693,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39044AD7-E24E-44ED-96F1-B34C34306CDC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -697,7 +733,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -709,7 +745,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -721,7 +757,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>